<commit_message>
Addition of frequencies to spreadsheet. Valdiation of alleles and strands.
</commit_message>
<xml_diff>
--- a/Tools/Snplists/T1D_GRS10/T1D_GRS10_1000G_nopalin_pos_hg19.xlsx
+++ b/Tools/Snplists/T1D_GRS10/T1D_GRS10_1000G_nopalin_pos_hg19.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/s_sharp_exeter_ac_uk/Documents/LIVE/hla-prs-toolkit/Snplists/T1D_GRS10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/s_sharp_exeter_ac_uk/Documents/LIVE/hla-prs-toolkit/Tools/Snplists/T1D_GRS10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_61F3AD472364FF18F55B1250EA5C713F8B303484" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2966E741-78D4-AF44-A060-5A555A7AAF91}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_61F3AD472364FF18F55B1250EA5C713F8B303484" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AF6AD74-497D-914D-BCA1-4504B9C7E4A9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="27120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18760" yWindow="940" windowWidth="25600" windowHeight="27120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="45">
   <si>
     <t>COMPONENT</t>
   </si>
@@ -42,12 +42,6 @@
     <t>REPLACING</t>
   </si>
   <si>
-    <t>A1_MAJOR</t>
-  </si>
-  <si>
-    <t>A2_MINOR</t>
-  </si>
-  <si>
     <t>POSITION_DBSNP151</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>SCORE_ALLELE</t>
   </si>
   <si>
-    <t>1000G?</t>
-  </si>
-  <si>
     <t>HLA-DQ25</t>
   </si>
   <si>
@@ -99,9 +90,6 @@
     <t>6:32671412</t>
   </si>
   <si>
-    <t>HLA</t>
-  </si>
-  <si>
     <t>rs3129889</t>
   </si>
   <si>
@@ -114,27 +102,18 @@
     <t>6:32413545</t>
   </si>
   <si>
-    <t>2.7</t>
-  </si>
-  <si>
     <t>rs2395029</t>
   </si>
   <si>
     <t>6:31431780</t>
   </si>
   <si>
-    <t>0.92</t>
-  </si>
-  <si>
     <t>rs1264813</t>
   </si>
   <si>
     <t>6:29939900</t>
   </si>
   <si>
-    <t>0.43</t>
-  </si>
-  <si>
     <t>NON-HLA</t>
   </si>
   <si>
@@ -144,9 +123,6 @@
     <t>1:114377568</t>
   </si>
   <si>
-    <t>0.67</t>
-  </si>
-  <si>
     <t>rs3842753</t>
   </si>
   <si>
@@ -162,25 +138,34 @@
     <t>10:6097283</t>
   </si>
   <si>
-    <t>0.46</t>
-  </si>
-  <si>
     <t>rs2292239</t>
   </si>
   <si>
     <t>12:56482180</t>
   </si>
   <si>
-    <t>0.3</t>
-  </si>
-  <si>
     <t>rs10509540</t>
   </si>
   <si>
     <t>10:90023033</t>
   </si>
   <si>
-    <t>0.29</t>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Freq_UKB(A1)</t>
+  </si>
+  <si>
+    <t>Freq_UKB(A2)</t>
+  </si>
+  <si>
+    <t>1000G_CHECKED?</t>
+  </si>
+  <si>
+    <t>HLA-Other</t>
   </si>
 </sst>
 </file>
@@ -221,9 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,375 +549,434 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="6" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
+      <c r="L1" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.854966</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.145034</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.89913100000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.100869</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F4" s="2">
+        <v>0.13966200000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.86033800000000005</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="J4" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="F5" s="2">
+        <v>0.96060800000000002</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3.9392000000000003E-2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.90452900000000003</v>
+      </c>
+      <c r="G6" s="2">
+        <v>9.5470700000000006E-2</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2">
+        <v>9.6524700000000005E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.90347500000000003</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.29438399999999998</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.70561600000000002</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.89375099999999996</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.106249</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.34439599999999998</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.65560399999999996</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.72569399999999995</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.27430599999999999</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="I11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="L12" s="1"/>
@@ -998,8 +1040,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:J1 A4:J7 A9:J11" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>